<commit_message>
import test file fixtures
</commit_message>
<xml_diff>
--- a/test/fixtures/files/Epi-X-Format-Invalid.xlsx
+++ b/test/fixtures/files/Epi-X-Format-Invalid.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/twong/Documents/SARA/SaraAlert/test/fixtures/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{703BB858-9726-CC4A-8051-6BB3EBB743A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDC4A842-0BA6-5E47-95B4-B9EC44563386}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2580" yWindow="2140" windowWidth="28800" windowHeight="13000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="80">
   <si>
     <t>DGMQ ID</t>
   </si>
@@ -190,433 +190,76 @@
     <t>China</t>
   </si>
   <si>
-    <t>MA</t>
-  </si>
-  <si>
-    <t>Boston</t>
-  </si>
-  <si>
-    <t>Abbott20</t>
-  </si>
-  <si>
-    <t>Billie79</t>
-  </si>
-  <si>
     <t>F</t>
   </si>
   <si>
-    <t>200 W Preston St</t>
-  </si>
-  <si>
     <t>BA2490</t>
   </si>
   <si>
     <t>EDV4886</t>
   </si>
   <si>
-    <t>GTI2688</t>
-  </si>
-  <si>
-    <t>CSN399</t>
-  </si>
-  <si>
-    <t>GTI7159</t>
-  </si>
-  <si>
-    <t>SVA3903</t>
-  </si>
-  <si>
-    <t>GEC8160</t>
-  </si>
-  <si>
-    <t>JBU1117</t>
-  </si>
-  <si>
     <t>Spanish</t>
   </si>
   <si>
-    <t>Korean</t>
-  </si>
-  <si>
-    <t>French</t>
-  </si>
-  <si>
-    <t>Chinese</t>
-  </si>
-  <si>
-    <t>German</t>
-  </si>
-  <si>
     <t>Portland</t>
   </si>
   <si>
     <t>Arlington</t>
   </si>
   <si>
-    <t>Medford</t>
-  </si>
-  <si>
-    <t>Bedford</t>
-  </si>
-  <si>
-    <t>Lexington</t>
-  </si>
-  <si>
-    <t>Quincy</t>
-  </si>
-  <si>
-    <t>Eugene</t>
-  </si>
-  <si>
-    <t>Dallas</t>
-  </si>
-  <si>
     <t>Balistreri67</t>
   </si>
   <si>
     <t>Tilda90</t>
   </si>
   <si>
-    <t>Bashirian28</t>
-  </si>
-  <si>
-    <t>Deshawn39</t>
-  </si>
-  <si>
-    <t>Beatty68</t>
-  </si>
-  <si>
-    <t>Jimmie77</t>
-  </si>
-  <si>
-    <t>Cole22</t>
-  </si>
-  <si>
-    <t>Loren79</t>
-  </si>
-  <si>
-    <t>Christiansen32</t>
-  </si>
-  <si>
-    <t>Ayako44</t>
-  </si>
-  <si>
-    <t>Jenkins69</t>
-  </si>
-  <si>
-    <t>Lashawn86</t>
-  </si>
-  <si>
-    <t>Kohler76</t>
-  </si>
-  <si>
-    <t>Darrel41</t>
-  </si>
-  <si>
     <t>M</t>
   </si>
   <si>
-    <t>205 W Preston St</t>
-  </si>
-  <si>
-    <t>209 W Preston St</t>
-  </si>
-  <si>
     <t>205 E Preston St</t>
   </si>
   <si>
-    <t>Peabody</t>
-  </si>
-  <si>
-    <t>Methuen</t>
-  </si>
-  <si>
-    <t>Austin</t>
-  </si>
-  <si>
-    <t>Little Rock</t>
-  </si>
-  <si>
-    <t>Atlanta</t>
-  </si>
-  <si>
-    <t>TX</t>
-  </si>
-  <si>
-    <t>32432-3234</t>
-  </si>
-  <si>
-    <t>53234-5290</t>
-  </si>
-  <si>
-    <t>03295-3243</t>
-  </si>
-  <si>
-    <t>01234</t>
-  </si>
-  <si>
     <t>1535997849fake@example.com</t>
   </si>
   <si>
-    <t>2535997849fake@example.com</t>
-  </si>
-  <si>
-    <t>153549fake@example.com</t>
-  </si>
-  <si>
-    <t>1534210123fake@example.com</t>
-  </si>
-  <si>
-    <t>112487912347fake@example.com</t>
-  </si>
-  <si>
-    <t>5732912fake@example.com</t>
-  </si>
-  <si>
-    <t>37289123fake@example.com</t>
-  </si>
-  <si>
-    <t>37294892fake@example.com</t>
-  </si>
-  <si>
     <t>Germany</t>
   </si>
   <si>
-    <t>Korea</t>
-  </si>
-  <si>
-    <t>Italy</t>
-  </si>
-  <si>
-    <t>Brazil</t>
-  </si>
-  <si>
-    <t>Domingo54</t>
-  </si>
-  <si>
     <t>EX-349212</t>
   </si>
   <si>
     <t>EX-499212</t>
   </si>
   <si>
-    <t>EX-349233</t>
-  </si>
-  <si>
-    <t>EX-349298</t>
-  </si>
-  <si>
-    <t>EX-123456</t>
-  </si>
-  <si>
-    <t>EX-329122</t>
-  </si>
-  <si>
-    <t>EX-345832</t>
-  </si>
-  <si>
-    <t>EX-312382</t>
-  </si>
-  <si>
-    <t>EX-789201</t>
-  </si>
-  <si>
-    <t>EX-910281</t>
-  </si>
-  <si>
-    <t>501 W Preston St</t>
-  </si>
-  <si>
-    <t>209 S Preston St</t>
-  </si>
-  <si>
-    <t>4403 Jessica Brook</t>
-  </si>
-  <si>
-    <t>509 Raymond Road Apt. 134</t>
-  </si>
-  <si>
-    <t>North Melany</t>
-  </si>
-  <si>
-    <t>AK</t>
-  </si>
-  <si>
-    <t>81536</t>
-  </si>
-  <si>
-    <t>3313 Jacobi Valleys</t>
-  </si>
-  <si>
-    <t>67386</t>
-  </si>
-  <si>
-    <t>Port Janel</t>
-  </si>
-  <si>
-    <t>NM</t>
-  </si>
-  <si>
-    <t>CA</t>
-  </si>
-  <si>
-    <t>North Wilsonland</t>
-  </si>
-  <si>
-    <t>28320-4417</t>
-  </si>
-  <si>
-    <t>73516 Weber Terrace</t>
-  </si>
-  <si>
-    <t>WV</t>
-  </si>
-  <si>
-    <t>Teresaville</t>
-  </si>
-  <si>
-    <t>47607</t>
-  </si>
-  <si>
-    <t>8676 Donn Mountains Apt. 618</t>
-  </si>
-  <si>
-    <t>Caryview</t>
-  </si>
-  <si>
-    <t>WA</t>
-  </si>
-  <si>
-    <t>AZ</t>
-  </si>
-  <si>
-    <t>18891</t>
-  </si>
-  <si>
-    <t>7624 Bayer Knolls</t>
-  </si>
-  <si>
-    <t>Leannonmouth</t>
-  </si>
-  <si>
-    <t>South Faustina</t>
-  </si>
-  <si>
-    <t>NV</t>
-  </si>
-  <si>
-    <t>39725-6840</t>
-  </si>
-  <si>
-    <t>2240 Adams Keys Suite 803</t>
-  </si>
-  <si>
-    <t>46750 Cremin Summit</t>
-  </si>
-  <si>
     <t>(555) 555-0111</t>
   </si>
   <si>
-    <t>(555) 555-0112</t>
-  </si>
-  <si>
-    <t>(555) 555-0113</t>
-  </si>
-  <si>
-    <t>(555) 555-0114</t>
-  </si>
-  <si>
-    <t>(555) 555-0115</t>
-  </si>
-  <si>
-    <t>(555) 555-0116</t>
-  </si>
-  <si>
-    <t>(555) 555-0119</t>
-  </si>
-  <si>
-    <t>(555) 555-0110</t>
-  </si>
-  <si>
-    <t>(555) 555-0123</t>
-  </si>
-  <si>
-    <t>(555) 555-0124</t>
-  </si>
-  <si>
     <t>Y</t>
   </si>
   <si>
-    <t>Natacha01</t>
-  </si>
-  <si>
-    <t>Batz96</t>
-  </si>
-  <si>
-    <t>Littel77</t>
-  </si>
-  <si>
-    <t>EX-886628</t>
-  </si>
-  <si>
-    <t>English</t>
-  </si>
-  <si>
-    <t>Piper83</t>
-  </si>
-  <si>
-    <t>Altenwerth99</t>
-  </si>
-  <si>
-    <t>7197 Johnson Dale</t>
-  </si>
-  <si>
-    <t>Irmaborough</t>
-  </si>
-  <si>
-    <t>SD</t>
-  </si>
-  <si>
-    <t>86846-7192</t>
-  </si>
-  <si>
-    <t>Oregon</t>
-  </si>
-  <si>
-    <t>Georgia</t>
-  </si>
-  <si>
-    <t>Vermont</t>
-  </si>
-  <si>
-    <t>2019-11-19</t>
-  </si>
-  <si>
-    <t>2020-01-06</t>
-  </si>
-  <si>
-    <t>2019-12-31</t>
-  </si>
-  <si>
-    <t>1965-09-08</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>YES</t>
-  </si>
-  <si>
-    <t>Yw</t>
-  </si>
-  <si>
     <t>yEs</t>
   </si>
   <si>
-    <t>YES!</t>
-  </si>
-  <si>
-    <t>yeah</t>
+    <t>asdfasf</t>
+  </si>
+  <si>
+    <t>asdvasd</t>
+  </si>
+  <si>
+    <t>asdfgba</t>
+  </si>
+  <si>
+    <t>asdbdsaf</t>
+  </si>
+  <si>
+    <t>asdfadsasd</t>
+  </si>
+  <si>
+    <t>asdfadasfd</t>
+  </si>
+  <si>
+    <t>asdfadsaf</t>
   </si>
 </sst>
 </file>
@@ -1445,9 +1088,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BC12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AG1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1665,10 +1306,10 @@
     </row>
     <row r="2" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>124</v>
+        <v>68</v>
       </c>
       <c r="B2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="E2">
         <v>5324</v>
@@ -1677,49 +1318,17 @@
         <v>43832</v>
       </c>
       <c r="J2" t="s">
-        <v>75</v>
-      </c>
-      <c r="K2" t="s">
-        <v>59</v>
-      </c>
-      <c r="L2" t="s">
-        <v>58</v>
-      </c>
-      <c r="M2" s="3">
-        <v>35996</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="M2" s="3"/>
       <c r="N2" t="s">
-        <v>60</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>61</v>
-      </c>
-      <c r="R2" t="s">
-        <v>57</v>
-      </c>
-      <c r="S2" t="s">
         <v>56</v>
       </c>
-      <c r="T2" s="5">
-        <v>21200</v>
-      </c>
-      <c r="U2" t="s">
-        <v>134</v>
-      </c>
-      <c r="V2" t="s">
-        <v>150</v>
-      </c>
-      <c r="W2" t="s">
-        <v>149</v>
-      </c>
-      <c r="X2" s="5" t="s">
-        <v>147</v>
-      </c>
       <c r="AC2" t="s">
-        <v>164</v>
+        <v>70</v>
       </c>
       <c r="AE2" s="6" t="s">
-        <v>111</v>
+        <v>66</v>
       </c>
       <c r="AI2" s="6"/>
       <c r="AJ2" t="s">
@@ -1729,557 +1338,126 @@
         <v>43829</v>
       </c>
       <c r="AP2" t="s">
-        <v>174</v>
+        <v>71</v>
       </c>
       <c r="AQ2" t="s">
-        <v>196</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>125</v>
+        <v>69</v>
       </c>
       <c r="B3" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C3" s="3"/>
       <c r="E3">
         <v>1249</v>
       </c>
       <c r="H3" t="s">
-        <v>70</v>
-      </c>
-      <c r="I3" s="3">
-        <v>43835</v>
+        <v>59</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>76</v>
       </c>
       <c r="J3" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="K3" t="s">
-        <v>83</v>
+        <v>62</v>
       </c>
       <c r="L3" t="s">
-        <v>84</v>
-      </c>
-      <c r="M3" s="3">
-        <v>34525</v>
+        <v>63</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>75</v>
       </c>
       <c r="N3" t="s">
-        <v>97</v>
+        <v>64</v>
       </c>
       <c r="Q3" t="s">
-        <v>100</v>
+        <v>65</v>
       </c>
       <c r="R3" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="S3" t="s">
-        <v>186</v>
-      </c>
-      <c r="T3" s="5">
-        <v>12345</v>
+        <v>73</v>
+      </c>
+      <c r="T3" s="5" t="s">
+        <v>74</v>
       </c>
       <c r="AC3" t="s">
-        <v>165</v>
+        <v>77</v>
       </c>
       <c r="AE3" s="6" t="s">
-        <v>112</v>
+        <v>78</v>
       </c>
       <c r="AJ3" t="s">
-        <v>119</v>
-      </c>
-      <c r="AK3" s="3">
-        <v>43831</v>
+        <v>67</v>
+      </c>
+      <c r="AK3" s="3" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:55" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>126</v>
-      </c>
-      <c r="B4" t="s">
-        <v>64</v>
-      </c>
-      <c r="E4">
-        <v>1821</v>
-      </c>
-      <c r="H4" t="s">
-        <v>71</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>190</v>
-      </c>
-      <c r="J4" t="s">
-        <v>77</v>
-      </c>
-      <c r="K4" t="s">
-        <v>85</v>
-      </c>
-      <c r="L4" t="s">
-        <v>86</v>
-      </c>
-      <c r="M4" s="3">
-        <v>36525</v>
-      </c>
-      <c r="N4" t="s">
-        <v>60</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>163</v>
-      </c>
-      <c r="R4" t="s">
-        <v>101</v>
-      </c>
-      <c r="S4" t="s">
-        <v>145</v>
-      </c>
-      <c r="T4" s="5">
-        <v>54321</v>
-      </c>
-      <c r="U4" t="s">
-        <v>148</v>
-      </c>
-      <c r="V4" t="s">
-        <v>146</v>
-      </c>
-      <c r="W4" t="s">
-        <v>155</v>
-      </c>
-      <c r="X4" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="AC4" t="s">
-        <v>166</v>
-      </c>
-      <c r="AD4" t="s">
-        <v>172</v>
-      </c>
-      <c r="AE4" s="6" t="s">
-        <v>113</v>
-      </c>
+      <c r="I4" s="5"/>
+      <c r="M4" s="3"/>
+      <c r="AE4" s="6"/>
       <c r="AK4" s="3"/>
-      <c r="AP4" t="s">
-        <v>193</v>
-      </c>
     </row>
     <row r="5" spans="1:55" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>127</v>
-      </c>
-      <c r="B5" t="s">
-        <v>65</v>
-      </c>
       <c r="C5" s="3"/>
-      <c r="E5">
-        <v>1842</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="J5" t="s">
-        <v>78</v>
-      </c>
-      <c r="K5" t="s">
-        <v>87</v>
-      </c>
-      <c r="L5" t="s">
-        <v>88</v>
-      </c>
-      <c r="M5" s="3">
-        <v>41279</v>
-      </c>
-      <c r="N5" t="s">
-        <v>60</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>152</v>
-      </c>
-      <c r="R5" t="s">
-        <v>153</v>
-      </c>
-      <c r="S5" t="s">
-        <v>154</v>
-      </c>
-      <c r="T5" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="AC5" t="s">
-        <v>167</v>
-      </c>
-      <c r="AD5" t="s">
-        <v>173</v>
-      </c>
-      <c r="AE5" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="AJ5" t="s">
-        <v>120</v>
-      </c>
-      <c r="AK5" s="3">
-        <v>43892</v>
-      </c>
-      <c r="AQ5" t="s">
-        <v>197</v>
-      </c>
+      <c r="I5" s="5"/>
+      <c r="M5" s="3"/>
+      <c r="AE5" s="6"/>
+      <c r="AK5" s="3"/>
     </row>
     <row r="6" spans="1:55" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>128</v>
-      </c>
-      <c r="B6" t="s">
-        <v>66</v>
-      </c>
       <c r="C6" s="3"/>
-      <c r="E6">
-        <v>1231</v>
-      </c>
-      <c r="H6" t="s">
-        <v>72</v>
-      </c>
-      <c r="I6" s="3">
-        <v>43788</v>
-      </c>
-      <c r="J6" t="s">
-        <v>79</v>
-      </c>
-      <c r="K6" t="s">
-        <v>89</v>
-      </c>
-      <c r="L6" t="s">
-        <v>90</v>
-      </c>
-      <c r="M6" s="3">
-        <v>42114</v>
-      </c>
-      <c r="N6" t="s">
-        <v>97</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>99</v>
-      </c>
-      <c r="R6" t="s">
-        <v>102</v>
-      </c>
-      <c r="S6" t="s">
-        <v>56</v>
-      </c>
-      <c r="T6" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="U6" t="s">
-        <v>135</v>
-      </c>
-      <c r="V6" t="s">
-        <v>158</v>
-      </c>
-      <c r="W6" t="s">
-        <v>188</v>
-      </c>
-      <c r="X6" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="AC6" t="s">
-        <v>168</v>
-      </c>
-      <c r="AE6" s="6" t="s">
-        <v>115</v>
-      </c>
+      <c r="I6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="AE6" s="6"/>
       <c r="AI6" s="6"/>
-      <c r="AJ6" t="s">
-        <v>121</v>
-      </c>
-      <c r="AK6" s="5" t="s">
-        <v>189</v>
-      </c>
+      <c r="AK6" s="5"/>
     </row>
     <row r="7" spans="1:55" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>129</v>
-      </c>
-      <c r="B7" t="s">
-        <v>67</v>
-      </c>
       <c r="C7" s="3"/>
-      <c r="E7">
-        <v>1242</v>
-      </c>
-      <c r="I7" s="3">
-        <v>43828</v>
-      </c>
-      <c r="J7" t="s">
-        <v>80</v>
-      </c>
-      <c r="K7" t="s">
-        <v>91</v>
-      </c>
-      <c r="L7" t="s">
-        <v>92</v>
-      </c>
-      <c r="M7" s="3">
-        <v>36331</v>
-      </c>
-      <c r="N7" t="s">
-        <v>97</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>141</v>
-      </c>
-      <c r="R7" t="s">
-        <v>103</v>
-      </c>
-      <c r="S7" t="s">
-        <v>106</v>
-      </c>
-      <c r="T7" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="AC7" t="s">
-        <v>169</v>
-      </c>
-      <c r="AE7" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="AP7" t="s">
-        <v>194</v>
-      </c>
+      <c r="I7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="AE7" s="6"/>
     </row>
     <row r="8" spans="1:55" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>130</v>
-      </c>
-      <c r="B8" t="s">
-        <v>68</v>
-      </c>
-      <c r="E8">
-        <v>6532</v>
-      </c>
-      <c r="H8" t="s">
-        <v>73</v>
-      </c>
-      <c r="I8" s="3">
-        <v>43833</v>
-      </c>
-      <c r="J8" t="s">
-        <v>81</v>
-      </c>
-      <c r="K8" t="s">
-        <v>175</v>
-      </c>
-      <c r="L8" t="s">
-        <v>176</v>
-      </c>
-      <c r="M8" s="3">
-        <v>27768</v>
-      </c>
-      <c r="N8" t="s">
-        <v>60</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>98</v>
-      </c>
-      <c r="R8" t="s">
-        <v>104</v>
-      </c>
-      <c r="S8" t="s">
-        <v>106</v>
-      </c>
-      <c r="T8" s="5">
-        <v>59321</v>
-      </c>
-      <c r="AE8" s="6" t="s">
-        <v>117</v>
-      </c>
+      <c r="I8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="AE8" s="6"/>
       <c r="AI8" s="6"/>
-      <c r="AJ8" t="s">
-        <v>122</v>
-      </c>
-      <c r="AK8" s="3">
-        <v>43895</v>
-      </c>
-      <c r="AQ8" t="s">
-        <v>198</v>
-      </c>
+      <c r="AK8" s="3"/>
     </row>
     <row r="9" spans="1:55" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>131</v>
-      </c>
-      <c r="B9" t="s">
-        <v>69</v>
-      </c>
-      <c r="E9">
-        <v>3482</v>
-      </c>
-      <c r="H9" t="s">
-        <v>74</v>
-      </c>
-      <c r="I9" s="3">
-        <v>43936</v>
-      </c>
-      <c r="J9" t="s">
-        <v>82</v>
-      </c>
-      <c r="K9" t="s">
-        <v>93</v>
-      </c>
-      <c r="L9" t="s">
-        <v>94</v>
-      </c>
-      <c r="M9" s="3">
-        <v>20142</v>
-      </c>
-      <c r="N9" t="s">
-        <v>97</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>162</v>
-      </c>
-      <c r="R9" t="s">
-        <v>105</v>
-      </c>
-      <c r="S9" t="s">
-        <v>187</v>
-      </c>
-      <c r="T9" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="AE9" s="6" t="s">
-        <v>118</v>
-      </c>
+      <c r="I9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="AE9" s="6"/>
     </row>
     <row r="10" spans="1:55" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>132</v>
-      </c>
       <c r="C10" s="3"/>
-      <c r="E10">
-        <v>2349</v>
-      </c>
-      <c r="I10" s="3">
-        <v>43960</v>
-      </c>
-      <c r="K10" t="s">
-        <v>177</v>
-      </c>
-      <c r="L10" t="s">
-        <v>123</v>
-      </c>
-      <c r="M10" s="5" t="s">
-        <v>192</v>
-      </c>
-      <c r="N10" t="s">
-        <v>60</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>137</v>
-      </c>
-      <c r="R10" t="s">
-        <v>138</v>
-      </c>
-      <c r="S10" t="s">
-        <v>139</v>
-      </c>
-      <c r="T10" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="U10" t="s">
-        <v>157</v>
-      </c>
-      <c r="V10" t="s">
-        <v>159</v>
-      </c>
-      <c r="W10" t="s">
-        <v>160</v>
-      </c>
-      <c r="X10" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="AC10" t="s">
-        <v>170</v>
-      </c>
-      <c r="AP10" t="s">
-        <v>195</v>
-      </c>
+      <c r="I10" s="3"/>
+      <c r="M10" s="5"/>
     </row>
     <row r="11" spans="1:55" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>133</v>
-      </c>
       <c r="I11" s="3"/>
-      <c r="K11" t="s">
-        <v>95</v>
-      </c>
-      <c r="L11" t="s">
-        <v>96</v>
-      </c>
-      <c r="M11" s="3">
-        <v>11747</v>
-      </c>
-      <c r="N11" t="s">
-        <v>97</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>136</v>
-      </c>
-      <c r="R11" t="s">
-        <v>143</v>
-      </c>
-      <c r="S11" t="s">
-        <v>144</v>
-      </c>
-      <c r="T11" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="AC11" t="s">
-        <v>171</v>
-      </c>
+      <c r="M11" s="3"/>
     </row>
     <row r="12" spans="1:55" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>178</v>
-      </c>
-      <c r="H12" t="s">
-        <v>179</v>
-      </c>
-      <c r="K12" t="s">
-        <v>181</v>
-      </c>
-      <c r="L12" t="s">
-        <v>180</v>
-      </c>
-      <c r="M12" s="3">
-        <v>38582</v>
-      </c>
-      <c r="N12" t="s">
-        <v>60</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>182</v>
-      </c>
-      <c r="R12" t="s">
-        <v>183</v>
-      </c>
-      <c r="S12" t="s">
-        <v>184</v>
-      </c>
-      <c r="T12" s="5" t="s">
-        <v>185</v>
-      </c>
+      <c r="M12" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="AE2" r:id="rId1" xr:uid="{D048A926-85A1-344B-9944-8309699DF8F0}"/>
-    <hyperlink ref="AE3" r:id="rId2" xr:uid="{6AA3A985-DC55-F44C-A035-93F5E054DB81}"/>
-    <hyperlink ref="AE4" r:id="rId3" xr:uid="{BFD701D4-F4B4-F64D-B6A2-060D573C32EA}"/>
-    <hyperlink ref="AE5" r:id="rId4" xr:uid="{B3639755-7E16-5A40-9922-8DF43D11D5B8}"/>
-    <hyperlink ref="AE6" r:id="rId5" xr:uid="{F1D1F5B2-13DD-014B-B6BB-BC21643B0F7E}"/>
-    <hyperlink ref="AE7" r:id="rId6" xr:uid="{CACA60BA-4ACA-3041-BF87-36EC887A68D9}"/>
-    <hyperlink ref="AE8" r:id="rId7" xr:uid="{E00EDE3E-9D61-4C46-A80A-3B8AC526092C}"/>
-    <hyperlink ref="AE9" r:id="rId8" xr:uid="{1D0308B9-1D8D-8C48-9AE1-056F656E4375}"/>
+    <hyperlink ref="AE3" r:id="rId2" display="2535997849fake@example.com" xr:uid="{6AA3A985-DC55-F44C-A035-93F5E054DB81}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-  <ignoredErrors>
-    <ignoredError sqref="T10:T11 T7 X4 X6" numberStoredAsText="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>